<commit_message>
função de excluir cliente funcionando
</commit_message>
<xml_diff>
--- a/Base de de dados (1).xlsx
+++ b/Base de de dados (1).xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,12 +473,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Correção</t>
+          <t>altteste</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SP</t>
+          <t>RS</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -487,24 +487,24 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>400000</v>
+        <v>500000</v>
       </c>
       <c r="E2" t="n">
-        <v>200000</v>
+        <v>75000</v>
       </c>
       <c r="F2" t="n">
-        <v>200000</v>
+        <v>425000</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>12/05/2022</t>
+          <t>30/02/2022</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>altteste</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -518,29 +518,29 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>500000</v>
+        <v>50000</v>
       </c>
       <c r="E3" t="n">
-        <v>75000</v>
+        <v>750000</v>
       </c>
       <c r="F3" t="n">
-        <v>425000</v>
+        <v>-700000</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>30/02/2022</t>
+          <t>30/12/2021</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>NEW</t>
+          <t>Teste Netflix</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>RS</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -552,167 +552,43 @@
         <v>50000</v>
       </c>
       <c r="E4" t="n">
-        <v>750000</v>
+        <v>80000</v>
       </c>
       <c r="F4" t="n">
-        <v>-700000</v>
+        <v>-30000</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>30/12/2021</t>
+          <t>12/02/2021</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>addteste</t>
+          <t>GUilhermee</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>go</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>br</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>25000</v>
+        <v>12000</v>
       </c>
       <c r="E5" t="n">
-        <v>26000</v>
+        <v>8500</v>
       </c>
       <c r="F5" t="n">
-        <v>-1000</v>
+        <v>3500</v>
       </c>
       <c r="G5" t="inlineStr">
-        <is>
-          <t>12/05/2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>nova adição</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>SC</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>BR</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>12000</v>
-      </c>
-      <c r="E6" t="n">
-        <v>7500</v>
-      </c>
-      <c r="F6" t="n">
-        <v>4500</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>12/02/2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Teste Netflix</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>SC</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>BR</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>50000</v>
-      </c>
-      <c r="E7" t="n">
-        <v>80000</v>
-      </c>
-      <c r="F7" t="n">
-        <v>-30000</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>12/02/2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>NOVO</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>SP</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>BR</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>12000</v>
-      </c>
-      <c r="E8" t="n">
-        <v>5000</v>
-      </c>
-      <c r="F8" t="n">
-        <v>7000</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>30/12/2022</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>GUilhermee</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>SP</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>BR</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>12000</v>
-      </c>
-      <c r="E9" t="n">
-        <v>8500</v>
-      </c>
-      <c r="F9" t="n">
-        <v>3500</v>
-      </c>
-      <c r="G9" t="inlineStr">
         <is>
           <t>12/12/2020</t>
         </is>

</xml_diff>

<commit_message>
Funcionalidade de alterar informação
</commit_message>
<xml_diff>
--- a/Base de de dados (1).xlsx
+++ b/Base de de dados (1).xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,7 +521,7 @@
         <v>50000</v>
       </c>
       <c r="E3" t="n">
-        <v>750000</v>
+        <v>50</v>
       </c>
       <c r="F3" t="n">
         <v>-700000</v>
@@ -593,6 +593,28 @@
           <t>12/12/2020</t>
         </is>
       </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>50</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
Revisão no layout das paginas
</commit_message>
<xml_diff>
--- a/Base de de dados (1).xlsx
+++ b/Base de de dados (1).xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -594,28 +594,6 @@
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="n">
-        <v>50</v>
-      </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
inicio da inclusaão do grafico
</commit_message>
<xml_diff>
--- a/Base de de dados (1).xlsx
+++ b/Base de de dados (1).xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,7 +524,7 @@
         <v>50</v>
       </c>
       <c r="F3" t="n">
-        <v>-700000</v>
+        <v>49950</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -591,6 +591,68 @@
       <c r="G5" t="inlineStr">
         <is>
           <t>12/12/2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Clinte</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>BR</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>20000</v>
+      </c>
+      <c r="E6" t="n">
+        <v>35000</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-15000</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>06/05/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Wen Tech</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>GO</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>BR</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="E7" t="n">
+        <v>900000</v>
+      </c>
+      <c r="F7" t="n">
+        <v>100000</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>12/12/2021</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Funcionalidade de busca de clientes
</commit_message>
<xml_diff>
--- a/Base de de dados (1).xlsx
+++ b/Base de de dados (1).xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,38 +497,36 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>addteste</t>
+          <t>Curly Armstrong</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>GO</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>25000</v>
+        <v>99849</v>
       </c>
       <c r="D2" t="n">
-        <v>26000</v>
+        <v>91557</v>
       </c>
       <c r="E2" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>12/05/2021</t>
-        </is>
+        <v>8292</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>44566</v>
       </c>
       <c r="G2" t="n">
-        <v>1000000</v>
+        <v>84628446067</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>PJ</t>
+          <t>PESSOA FISICA</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>199052902</v>
+        <v>19982458754</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -540,38 +542,36 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Correção</t>
+          <t>Cliff Barker</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SP</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>400000</v>
+        <v>80319</v>
       </c>
       <c r="D3" t="n">
-        <v>200000</v>
+        <v>54772</v>
       </c>
       <c r="E3" t="n">
-        <v>200000</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>12/05/2022</t>
-        </is>
+        <v>25547</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>44566</v>
       </c>
       <c r="G3" t="n">
-        <v>15505150</v>
+        <v>84628446068</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>PESSOA FISICA</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>165188152</v>
+        <v>19982458755</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -587,38 +587,36 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Lebron James</t>
+          <t>Leo Barnhorst</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>GO</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>10000</v>
+        <v>91480</v>
       </c>
       <c r="D4" t="n">
-        <v>8000</v>
+        <v>54686</v>
       </c>
       <c r="E4" t="n">
-        <v>2000</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>12/05/2022</t>
-        </is>
+        <v>36794</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>44566</v>
       </c>
       <c r="G4" t="n">
-        <v>15646152</v>
+        <v>84628446069</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>PJ</t>
+          <t>PESSOA FISICA</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>165121832</v>
+        <v>19982458756</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -634,38 +632,36 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ALTTESTE</t>
+          <t>Ed Bartels</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>RS</t>
+          <t>MT</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>50000</v>
+        <v>59779</v>
       </c>
       <c r="D5" t="n">
-        <v>750000</v>
+        <v>89793</v>
       </c>
       <c r="E5" t="n">
-        <v>-700000</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>25/12/2022</t>
-        </is>
+        <v>-30014</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>44566</v>
       </c>
       <c r="G5" t="n">
-        <v>26854648</v>
+        <v>84628446070</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>PESSOA FISICA</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>165512185</v>
+        <v>19982458757</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -681,38 +677,36 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>sorveteiros FC</t>
+          <t>Ralph Beard</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CF</t>
+          <t>RS</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>50000</v>
+        <v>92061</v>
       </c>
       <c r="D6" t="n">
-        <v>7500</v>
+        <v>20015</v>
       </c>
       <c r="E6" t="n">
-        <v>42500</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>25/12/2022</t>
-        </is>
+        <v>72046</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>44566</v>
       </c>
       <c r="G6" t="n">
-        <v>15615125</v>
+        <v>84628446071</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>PJ</t>
+          <t>PESSOA FISICA</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>165123518</v>
+        <v>19982458758</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -728,38 +722,36 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>altteste</t>
+          <t>Gene Berce</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>RS</t>
+          <t>ES</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>500000</v>
+        <v>25989</v>
       </c>
       <c r="D7" t="n">
-        <v>75000</v>
+        <v>49680</v>
       </c>
       <c r="E7" t="n">
-        <v>425000</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>30/02/2023</t>
-        </is>
+        <v>-23691</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>44566</v>
       </c>
       <c r="G7" t="n">
-        <v>13541511</v>
+        <v>84628446072</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>PESSOA FISICA</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1651265123</v>
+        <v>19982458759</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -775,7 +767,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>NOVO CLIENTE</t>
+          <t>Charlie Black</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -784,21 +776,19 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>500000</v>
+        <v>98486</v>
       </c>
       <c r="D8" t="n">
-        <v>17500</v>
+        <v>69556</v>
       </c>
       <c r="E8" t="n">
-        <v>2500</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>12/05/2021</t>
-        </is>
+        <v>28930</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>44566</v>
       </c>
       <c r="G8" t="n">
-        <v>1000010101</v>
+        <v>84628446073</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -806,16 +796,1096 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1998289845</v>
+        <v>19982458760</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>TATATA@GMAIL.COM</t>
+          <t>email@email</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Nelson Bobb</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>73679</v>
+      </c>
+      <c r="D9" t="n">
+        <v>63149</v>
+      </c>
+      <c r="E9" t="n">
+        <v>10530</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>44566</v>
+      </c>
+      <c r="G9" t="n">
+        <v>84628446074</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>PESSOA FISICA</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>19982458761</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
           <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Jake Bornheimer</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>GO</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>57141</v>
+      </c>
+      <c r="D10" t="n">
+        <v>71963</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-14822</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>44566</v>
+      </c>
+      <c r="G10" t="n">
+        <v>84628446075</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>PESSOA FISICA</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>19982458762</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Vince Boryla</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>MT</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>24571</v>
+      </c>
+      <c r="D11" t="n">
+        <v>24623</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-52</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>44566</v>
+      </c>
+      <c r="G11" t="n">
+        <v>84628446076</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>PESSOA FISICA</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>19982458763</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Don Boven</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>RS</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>60354</v>
+      </c>
+      <c r="D12" t="n">
+        <v>43097</v>
+      </c>
+      <c r="E12" t="n">
+        <v>17257</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>44566</v>
+      </c>
+      <c r="G12" t="n">
+        <v>84628446077</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>PESSOA FISICA</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>19982458764</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Harry Boykoff</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ES</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>34081</v>
+      </c>
+      <c r="D13" t="n">
+        <v>64921</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-30840</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>44566</v>
+      </c>
+      <c r="G13" t="n">
+        <v>84628446078</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>PESSOA FISICA</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>19982458765</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Joe Bradley</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>80560</v>
+      </c>
+      <c r="D14" t="n">
+        <v>24150</v>
+      </c>
+      <c r="E14" t="n">
+        <v>56410</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>44566</v>
+      </c>
+      <c r="G14" t="n">
+        <v>17929691000105</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>PESSOA JURIDICA</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>19982458766</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Bob Brannum</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>99593</v>
+      </c>
+      <c r="D15" t="n">
+        <v>93531</v>
+      </c>
+      <c r="E15" t="n">
+        <v>6062</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>44566</v>
+      </c>
+      <c r="G15" t="n">
+        <v>17929691000106</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>PESSOA JURIDICA</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>19982458767</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Carl Braun</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>41235</v>
+      </c>
+      <c r="D16" t="n">
+        <v>87530</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-46295</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>44566</v>
+      </c>
+      <c r="G16" t="n">
+        <v>17929691000107</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>PESSOA JURIDICA</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>19982458768</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Frankie Brian</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>94512</v>
+      </c>
+      <c r="D17" t="n">
+        <v>78201</v>
+      </c>
+      <c r="E17" t="n">
+        <v>16311</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>44566</v>
+      </c>
+      <c r="G17" t="n">
+        <v>17929691000108</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>PESSOA JURIDICA</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>19982458769</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Price Brookfield</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>GO</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>56690</v>
+      </c>
+      <c r="D18" t="n">
+        <v>76974</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-20284</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>44567</v>
+      </c>
+      <c r="G18" t="n">
+        <v>17929691000109</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>PESSOA JURIDICA</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>19982458770</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Bob Brown</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>MT</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>31738</v>
+      </c>
+      <c r="D19" t="n">
+        <v>40986</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-9248</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>44568</v>
+      </c>
+      <c r="G19" t="n">
+        <v>17929691000110</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>PESSOA JURIDICA</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>19982458771</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Jim Browne</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>RS</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>67663</v>
+      </c>
+      <c r="D20" t="n">
+        <v>88920</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-21257</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>44569</v>
+      </c>
+      <c r="G20" t="n">
+        <v>17929691000111</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>PESSOA JURIDICA</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>19982458772</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Walt Budko</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ES</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>89421</v>
+      </c>
+      <c r="D21" t="n">
+        <v>91396</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-1975</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>44570</v>
+      </c>
+      <c r="G21" t="n">
+        <v>17929691000112</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>PESSOA JURIDICA</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>19982458773</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Jack Burmaster</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>28572</v>
+      </c>
+      <c r="D22" t="n">
+        <v>88574</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-60002</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>44571</v>
+      </c>
+      <c r="G22" t="n">
+        <v>17929691000113</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>PESSOA JURIDICA</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>19982458774</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Tommy Byrnes</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>38529</v>
+      </c>
+      <c r="D23" t="n">
+        <v>59069</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-20540</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <v>44567</v>
+      </c>
+      <c r="G23" t="n">
+        <v>17929691000114</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>PESSOA JURIDICA</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>19982458775</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Bill Calhoun</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>GO</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>53712</v>
+      </c>
+      <c r="D24" t="n">
+        <v>94365</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-40653</v>
+      </c>
+      <c r="F24" s="2" t="n">
+        <v>44568</v>
+      </c>
+      <c r="G24" t="n">
+        <v>17929691000115</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>PESSOA JURIDICA</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>19982458776</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Don Carlson</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>MT</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>90137</v>
+      </c>
+      <c r="D25" t="n">
+        <v>39020</v>
+      </c>
+      <c r="E25" t="n">
+        <v>51117</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <v>44569</v>
+      </c>
+      <c r="G25" t="n">
+        <v>17929691000116</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>PESSOA JURIDICA</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>19982458777</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Bob Carpenter</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>RS</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>88489</v>
+      </c>
+      <c r="D26" t="n">
+        <v>32553</v>
+      </c>
+      <c r="E26" t="n">
+        <v>55936</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <v>44570</v>
+      </c>
+      <c r="G26" t="n">
+        <v>17929691000117</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>PESSOA JURIDICA</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>19982458778</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Jake Carter</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ES</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>30716</v>
+      </c>
+      <c r="D27" t="n">
+        <v>66646</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-35930</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>44571</v>
+      </c>
+      <c r="G27" t="n">
+        <v>17929691000118</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>PESSOA JURIDICA</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>19982458779</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Al Cervi*</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>58919</v>
+      </c>
+      <c r="D28" t="n">
+        <v>80208</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-21289</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>44567</v>
+      </c>
+      <c r="G28" t="n">
+        <v>17929691000119</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>PESSOA JURIDICA</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>19982458780</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>John Chaney</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>62869</v>
+      </c>
+      <c r="D29" t="n">
+        <v>58474</v>
+      </c>
+      <c r="E29" t="n">
+        <v>4395</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>44568</v>
+      </c>
+      <c r="G29" t="n">
+        <v>17929691000120</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>PESSOA JURIDICA</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>19982458781</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Leroy Chollet</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>25359</v>
+      </c>
+      <c r="D30" t="n">
+        <v>46139</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-20780</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <v>44569</v>
+      </c>
+      <c r="G30" t="n">
+        <v>17929691000121</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>PESSOA JURIDICA</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>19982458782</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Bill Closs</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>89581</v>
+      </c>
+      <c r="D31" t="n">
+        <v>65293</v>
+      </c>
+      <c r="E31" t="n">
+        <v>24288</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>44570</v>
+      </c>
+      <c r="G31" t="n">
+        <v>17929691000122</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>PESSOA JURIDICA</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>19982458783</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Paul Cloyd</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>GO</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>78293</v>
+      </c>
+      <c r="D32" t="n">
+        <v>58593</v>
+      </c>
+      <c r="E32" t="n">
+        <v>19700</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <v>44571</v>
+      </c>
+      <c r="G32" t="n">
+        <v>17929691000123</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>PESSOA JURIDICA</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>19982458784</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>email@email</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>A</t>
         </is>
       </c>
     </row>

</xml_diff>